<commit_message>
Tidsplan revideret + pdf
</commit_message>
<xml_diff>
--- a/Administration/Tidsplan 1.0.xlsx
+++ b/Administration/Tidsplan 1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Desktop\Ultralyds-Robotarm-4SEMPRJ\Bilag - diverse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anne\Desktop\Ultralyds-Robotarm-4SEMPRJ\Administration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -522,6 +522,7 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -543,7 +544,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -866,7 +866,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -879,53 +879,53 @@
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23">
+      <c r="B1" s="24">
         <v>2015</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="26"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27" t="s">
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="27" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="29"/>
+      <c r="P2" s="28"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="30"/>
     </row>
     <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
@@ -1032,16 +1032,16 @@
         <v>27</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="30"/>
+      <c r="C6" s="23"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
@@ -1282,10 +1282,10 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
       <c r="K17" s="17"/>
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
@@ -1357,11 +1357,11 @@
       <c r="K20" s="21"/>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
-      <c r="N20" s="30"/>
-      <c r="O20" s="30"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="17"/>
-      <c r="R20" s="2"/>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
@@ -1379,11 +1379,11 @@
       <c r="K21" s="21"/>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
       <c r="Q21" s="17"/>
-      <c r="R21" s="2"/>
+      <c r="R21" s="18"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
@@ -1440,6 +1440,6 @@
     <mergeCell ref="O2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>